<commit_message>
write data to table
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -32,11 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00&quot; PLN&quot;"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -401,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -430,55 +428,78 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>44896</v>
-      </c>
-      <c r="B2" s="1">
-        <v>215.99</v>
+      <c r="A2" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>бригады</v>
+        <v>Бригада</v>
       </c>
       <c r="D2" s="1" t="str">
-        <v>имя фамилия</v>
+        <v/>
       </c>
       <c r="E2" s="1" t="str">
-        <v>топливо</v>
+        <v>Материал</v>
       </c>
       <c r="F2" s="1" t="str">
-        <v>объект</v>
+        <v>Skysawa</v>
       </c>
       <c r="G2" s="1" t="str">
-        <v>Бригада Игоря</v>
+        <v>Бригада Миши</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>44896</v>
-      </c>
-      <c r="B3" s="1">
-        <v>215.99</v>
+      <c r="A3" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <v>23.69</v>
       </c>
       <c r="C3" s="1" t="str">
-        <v>бригады</v>
+        <v>Люди</v>
       </c>
       <c r="D3" s="1" t="str">
-        <v>Алеша Поповч</v>
+        <v/>
       </c>
       <c r="E3" s="1" t="str">
-        <v>мозги</v>
+        <v>Почта</v>
       </c>
       <c r="F3" s="1" t="str">
-        <v>Кудыкина гора</v>
+        <v>Office</v>
       </c>
       <c r="G3" s="1" t="str">
-        <v>Бригада Святослава Ярополковича</v>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <v>Андрей - керовник</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <v>Почта</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G37"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write to table menu
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -519,10 +519,608 @@
         <v/>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E6" s="1" t="str">
+        <v>Топливо</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <v>Бригада Игоря</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <v>123</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <v>Александра</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <v>Инструмент</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <v>123</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E8" s="1" t="str">
+        <v>Зарплата</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <v>Skysawa</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <v>205</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <v>Zyben Mikhail</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <v>Зарплата</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <v>Владислав</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <v>Страховки на авто</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <v>300</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <v>Андрей - керовник</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <v>Аванс</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <v>Skysawa</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <v>563</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <v>199,9</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E13" s="1" t="str">
+        <v>Топливо</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <v>Бригада Игоря</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <v>458</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E14" s="1" t="str">
+        <v>Ксеро</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <v>Shartukh Anton i Aliaksandr</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E15" s="1" t="str">
+        <v>Аванс</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <v>Бригада Миши</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <v>589</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <v>Lelyuk Alexandr</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <v>Зарплата</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <v>Novisa</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <v>Бригада Лелюка</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <v>541</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <v>Валерий</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <v>Зарплата</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <v>Novisa</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <v>Shartukh Anton i Aliaksandr</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <v>589</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <v>Андрийко</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <v>Материал</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <v>GIPS Karpacz</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <v>542</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <v>Tsishkou Dmitry</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <v>Страховки на авто</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <v>Shartukh Anton i Aliaksandr</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <v>523</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E20" s="1" t="str">
+        <v>Страховки на авто</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <v>Shartukh Anton i Aliaksandr</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <v>586</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <v>Statsenka Aliaksandr</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <v>Почта</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <v>589</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E22" s="1" t="str">
+        <v>Почта</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <v>Novisa</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <v>Mykola i Oleksii</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <v>589</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E23" s="1" t="str">
+        <v>Ксеро</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <v>Novisa</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <v>Бригада Игоря</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <v>200,05</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <v>Богдан</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <v>54,5</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <v>Tarasiuk Oleksandr</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <v>Ксеро</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <v>589</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <v>Koushyk Petr</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <v>Ксеро</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <v>52.3</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <v>Андрийко</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <v>Ксеро</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <v>52.6</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E28" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <v>Бригада Лелюка</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <v>52.6</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <v>Dranyk Oleksandr</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <v>Ксеро</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G29" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <v>4.36</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <v>Statsenka Aliaksandr</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <v>Ксеро</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="str">
+        <v>09.11.2022</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <v>5.36</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E31" s="1" t="str">
+        <v>Почта</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
isAdmin func; get table func
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -429,100 +429,54 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>09.11.2022</v>
+        <v>10.11.2022</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>52,6</v>
+        <v>25,36</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>Бригада</v>
+        <v>Общее</v>
       </c>
       <c r="D2" s="1" t="str">
         <v/>
       </c>
       <c r="E2" s="1" t="str">
-        <v>Почта</v>
+        <v>Ксеро</v>
       </c>
       <c r="F2" s="1" t="str">
-        <v>Skysawa</v>
+        <v>Karpacz</v>
       </c>
       <c r="G2" s="1" t="str">
-        <v>Бригада Миши</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <v>09.11.2022</v>
+        <v>10.11.2022</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v>52,69</v>
+        <v>215</v>
       </c>
       <c r="C3" s="1" t="str">
-        <v>Бригада</v>
+        <v>Люди</v>
       </c>
       <c r="D3" s="1" t="str">
-        <v/>
+        <v>Владислав</v>
       </c>
       <c r="E3" s="1" t="str">
-        <v>Материал</v>
+        <v>Топливо</v>
       </c>
       <c r="F3" s="1" t="str">
-        <v>Karpacz</v>
+        <v>Office</v>
       </c>
       <c r="G3" s="1" t="str">
-        <v>Бригада Миши</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="str">
-        <v>09.11.2022</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <v>214,69</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <v>Люди</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <v>Lelyuk Alexandr</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <v>Аванс</v>
-      </c>
-      <c r="F4" s="1" t="str">
-        <v>GIPS Karpacz</v>
-      </c>
-      <c r="G4" s="1" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="str">
-        <v>09.11.2022</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <v>523,8</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <v>Общее</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <v/>
-      </c>
-      <c r="E5" s="1" t="str">
-        <v>Топливо</v>
-      </c>
-      <c r="F5" s="1" t="str">
-        <v>Office</v>
-      </c>
-      <c r="G5" s="1" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chenhe res obj; add workheet head, col width
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -399,32 +399,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="str">
-        <v>дата</v>
+        <v>Дата</v>
       </c>
       <c r="B1" s="1" t="str">
-        <v>сумма</v>
+        <v>Сумма</v>
       </c>
       <c r="C1" s="1" t="str">
-        <v>вид</v>
+        <v>Вид</v>
       </c>
       <c r="D1" s="1" t="str">
-        <v>люди</v>
+        <v>Люди</v>
       </c>
       <c r="E1" s="1" t="str">
-        <v>титул</v>
+        <v>Титул</v>
       </c>
       <c r="F1" s="1" t="str">
-        <v>объект</v>
+        <v>Объект</v>
       </c>
       <c r="G1" s="1" t="str">
-        <v>бригады</v>
+        <v>Бригады</v>
       </c>
     </row>
     <row r="2">
@@ -432,22 +441,22 @@
         <v>10.11.2022</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>25,36</v>
+        <v>253,6</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>Общее</v>
+        <v>Бригада</v>
       </c>
       <c r="D2" s="1" t="str">
         <v/>
       </c>
       <c r="E2" s="1" t="str">
-        <v>Ксеро</v>
+        <v>Аванс</v>
       </c>
       <c r="F2" s="1" t="str">
-        <v>Karpacz</v>
+        <v>MCM project</v>
       </c>
       <c r="G2" s="1" t="str">
-        <v/>
+        <v>Shartukh Anton i Aliaksandr</v>
       </c>
     </row>
     <row r="3">
@@ -455,28 +464,74 @@
         <v>10.11.2022</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v>215</v>
+        <v>23,69</v>
       </c>
       <c r="C3" s="1" t="str">
         <v>Люди</v>
       </c>
       <c r="D3" s="1" t="str">
-        <v>Владислав</v>
+        <v>Tarasiuk Oleksandr</v>
       </c>
       <c r="E3" s="1" t="str">
+        <v>Страховки на авто</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <v>Skysawa</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="str">
+        <v>10.11.2022</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <v>25,36</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E4" s="1" t="str">
+        <v>Зарплата</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="str">
+        <v>10.11.2022</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <v>25,69</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <v>Анастасия PM</v>
+      </c>
+      <c r="E5" s="1" t="str">
         <v>Топливо</v>
       </c>
-      <c r="F3" s="1" t="str">
+      <c r="F5" s="1" t="str">
         <v>Office</v>
       </c>
-      <c r="G3" s="1" t="str">
+      <c r="G5" s="1" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stop btn, fix isAdmin, write user info
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -528,10 +528,263 @@
         <v/>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E6" s="1" t="str">
+        <v>Топливо</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <v>Novisa</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E7" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <v>Бригада Лелюка</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E8" s="1" t="str">
+        <v>Топливо</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <v>Skysawa</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <v>Бригада Миши</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <v>Lelyuk Alexandr</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <v>Материал</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <v>53,89</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="1" t="str">
+        <v>Топливо</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <v>32,78</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="1" t="str">
+        <v>Проезд - билеты</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <v>43,98</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="1" t="str">
+        <v>Инструмент</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <v>23,69</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E13" s="1" t="str">
+        <v>Зарплата</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <v>214,36</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E14" s="1" t="str">
+        <v>коллекция покемонов</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="str">
+        <v>17.11.2022</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <v>Бригада</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E15" s="1" t="str">
+        <v>Габилен</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <v>Бригада Игоря</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="str">
+        <v>19.11.2022</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <v>43,89</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <v>Люди</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <v>Владислав</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
header table fix; date fix; sen msg info;comment add
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -435,6 +435,12 @@
       <c r="G1" s="1" t="str">
         <v>Бригады</v>
       </c>
+      <c r="H1" s="1" t="str">
+        <v>ФИО</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <v>Комментарий</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
@@ -781,10 +787,377 @@
         <v/>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="str">
+        <v>19.11.2022</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <v>65,88</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E17" s="1" t="str">
+        <v>Материал</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <v>Skysawa</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="str">
+        <v>19.11.2022</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <v>25,3</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E18" s="1" t="str">
+        <v>что-нибудь такое</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E19" s="1" t="str">
+        <v>Материал</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <v>Skysawa</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H19" s="1" t="str">
+        <v>Rybkin Anton</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E20" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H20" s="1" t="str">
+        <v>Rybkin Anton | s_ryb</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <v>255</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E21" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H21" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <v>2569</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E22" s="1" t="str">
+        <v>Дичь собачья</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <v>Office</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H22" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <v>256</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E23" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <v>GIPS Karpacz</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H23" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <v>214</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E24" s="1" t="str">
+        <v>Топливо</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H24" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <v>548</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E25" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H25" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <v>548</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E26" s="1" t="str">
+        <v>Жилье</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H26" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <v>548</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E27" s="1" t="str">
+        <v>Расходники</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H27" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <v>548</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E28" s="1" t="str">
+        <v>Расходники</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <v>MCM project</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H28" s="1" t="str">
+        <v>Rybkin Anton; s_ryb; 192713235</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <v>ну типа того вот так и эдак</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <v>4123</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E29" s="1" t="str">
+        <v>Топливо</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <v>Karpacz</v>
+      </c>
+      <c r="G29" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H29" s="1" t="str">
+        <v>Rybkin Anton; s_ryb</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <v>шла саша по шосе и сосала сушку</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="str">
+        <v>20.12.2022</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <v>589</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <v>Общее</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E30" s="1" t="str">
+        <v>херня какая-то</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <v>GIPS Karpacz</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H30" s="1" t="str">
+        <v>Rybkin Anton; s_ryb</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <v>нужная херня очень</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I30"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>